<commit_message>
Applicants and Interview details
</commit_message>
<xml_diff>
--- a/makerclan/projects/ELRMD059043/ELRMD059043.xlsx
+++ b/makerclan/projects/ELRMD059043/ELRMD059043.xlsx
@@ -58,7 +58,7 @@
     <t>flag</t>
   </si>
   <si>
-    <t>2018-02-16</t>
+    <t>2018-03-10</t>
   </si>
 </sst>
 </file>
@@ -419,7 +419,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>